<commit_message>
Feat: Show MaxAttackRange Decal
A키를 누르면 직업마다 다른 최대공격 사거리를 볼 수 있도록 데칼이 나타납니다.
토글처럼 한번 만들면 껐다 키는 느낌으로 설정했습니다.
</commit_message>
<xml_diff>
--- a/GameData/GOCharacterStatTable.xlsx
+++ b/GameData/GOCharacterStatTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Epic Games\UE_5.3\GuardiansOrders\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EC2CDE-958A-447F-A6C6-01B61CB28725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5144F32-0516-44F8-A1D3-59AC192A30DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="12560" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GOCharacterStatTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>MaxHP</t>
   </si>
@@ -77,6 +77,10 @@
   </si>
   <si>
     <t>HpRegenerationRate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxBasicAttackRange</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1041,7 +1045,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -1052,15 +1056,16 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9.75" customWidth="1"/>
-    <col min="10" max="10" width="22.4140625" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="9.75" customWidth="1"/>
+    <col min="11" max="11" width="22.4140625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1074,28 +1079,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1109,28 +1117,31 @@
         <v>300</v>
       </c>
       <c r="E2" s="1">
+        <v>75</v>
+      </c>
+      <c r="F2" s="1">
         <v>25</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>75</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>100</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>25</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>200</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>2</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1144,28 +1155,31 @@
         <v>400</v>
       </c>
       <c r="E3" s="1">
+        <v>350</v>
+      </c>
+      <c r="F3" s="1">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>350</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>25</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>50</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>250</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>4</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1179,28 +1193,31 @@
         <v>330</v>
       </c>
       <c r="E4" s="1">
+        <v>150</v>
+      </c>
+      <c r="F4" s="1">
         <v>80</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>150</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>75</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>35</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>225</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1214,24 +1231,27 @@
         <v>370</v>
       </c>
       <c r="E5" s="1">
+        <v>250</v>
+      </c>
+      <c r="F5" s="1">
         <v>40</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>250</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>150</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>30</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>300</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>5</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>25</v>
       </c>
     </row>

</xml_diff>